<commit_message>
UN SDGs taxonomy added
</commit_message>
<xml_diff>
--- a/taxonomy4good/taxonomies/china_taxonomy.xlsx
+++ b/taxonomy4good/taxonomies/china_taxonomy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anis.bouhamadouche/PycharmProjects/taxonomy4good/taxonomy4good/taxonomies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F04F06-FC95-7945-AC1B-B36D5FDB8803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B0C871-E66E-9A48-AA77-B30AF6F5B285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1390,5 +1390,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>